<commit_message>
=error cleared in excel import
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -61,7 +61,7 @@
     <t>test@mail.com</t>
   </si>
   <si>
-    <t>dfdfd</t>
+    <t>check</t>
   </si>
 </sst>
 </file>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,20 +511,6 @@
         <v>8464646</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H3" s="3"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H4" s="3"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H6" s="3"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>

</xml_diff>